<commit_message>
add loginFilter when ignore player's request when he's not logined
</commit_message>
<xml_diff>
--- a/gameData/shared/PlayerInitData.xlsx
+++ b/gameData/shared/PlayerInitData.xlsx
@@ -4,26 +4,31 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="22900" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="2"/>
+    <workbookView xWindow="5620" yWindow="22280" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="resources" sheetId="2" r:id="rId1"/>
     <sheet name="materials" sheetId="15" r:id="rId2"/>
     <sheet name="soldierMaterials" sheetId="19" r:id="rId3"/>
-    <sheet name="houses" sheetId="18" r:id="rId4"/>
+    <sheet name="dragonMaterials" sheetId="20" r:id="rId4"/>
+    <sheet name="houses" sheetId="18" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="3">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="3">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="3">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="3">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8">#REF!</definedName>
   </definedNames>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -175,6 +180,154 @@
   </si>
   <si>
     <t>INT_brightAlloy</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_ironIngot</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_steelIngot</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_mithrilIngot</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_blackIronIngot</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_arcaniteIngot</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_wispOfFire</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_wispOfCold</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_wispOfWind</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_lavaSoul</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_iceSoul</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_forestSoul</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_infernoSoul</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_blizzardSoul</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_fairySoul</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_moltenShard</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_glacierShard</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_chargedShard</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_moltenShiver</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_glacierShiver</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_chargedShiver</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_moltenCore</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_glacierCore</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_chargedCore</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_moltenMagnet</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_glacierMagnet</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_chargedMagnet</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_challengeRune</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_suppressRune</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_rageRune</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_guardRune</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_poisonRune</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_giantRune</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_dolanRune</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_warsongRune</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_infernoRune</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_arcanaRune</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_eternityRune</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1044,7 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -1124,6 +1277,263 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="20.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" s="3" customFormat="1" ht="20" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="20" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>

</xml_diff>

<commit_message>
finish dev of player townhall
</commit_message>
<xml_diff>
--- a/gameData/shared/PlayerInitData.xlsx
+++ b/gameData/shared/PlayerInitData.xlsx
@@ -4,58 +4,53 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="5780" windowWidth="27520" windowHeight="14540" tabRatio="883" activeTab="8"/>
+    <workbookView xWindow="7800" yWindow="4920" windowWidth="27520" windowHeight="14540" tabRatio="883"/>
   </bookViews>
   <sheets>
-    <sheet name="resources" sheetId="2" r:id="rId1"/>
-    <sheet name="materials" sheetId="15" r:id="rId2"/>
-    <sheet name="soldierMaterials" sheetId="19" r:id="rId3"/>
-    <sheet name="dragonMaterials" sheetId="20" r:id="rId4"/>
-    <sheet name="houses" sheetId="18" r:id="rId5"/>
-    <sheet name="playerLevel" sheetId="21" r:id="rId6"/>
-    <sheet name="vipLevel" sheetId="22" r:id="rId7"/>
-    <sheet name="collectLevel" sheetId="23" r:id="rId8"/>
-    <sheet name="dailyQuests" sheetId="24" r:id="rId9"/>
-    <sheet name="dailyQuestStar" sheetId="25" r:id="rId10"/>
-    <sheet name="dailyQuestStyle" sheetId="26" r:id="rId11"/>
+    <sheet name="intInit" sheetId="24" r:id="rId1"/>
+    <sheet name="floatInit" sheetId="25" r:id="rId2"/>
+    <sheet name="resources" sheetId="2" r:id="rId3"/>
+    <sheet name="materials" sheetId="15" r:id="rId4"/>
+    <sheet name="soldierMaterials" sheetId="19" r:id="rId5"/>
+    <sheet name="dragonMaterials" sheetId="20" r:id="rId6"/>
+    <sheet name="houses" sheetId="18" r:id="rId7"/>
+    <sheet name="playerLevel" sheetId="21" r:id="rId8"/>
+    <sheet name="vipLevel" sheetId="22" r:id="rId9"/>
+    <sheet name="collectLevel" sheetId="23" r:id="rId10"/>
   </sheets>
   <definedNames>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="9">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="1">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="7">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="9">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="10">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="1">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="5">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="2">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="8">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="9">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="1">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="6">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="7">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="9">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="10">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="5">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="2">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="8">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="9">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="1">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="6">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="7">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="9">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="10">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="5">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="2">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="8">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="9">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="1">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="6">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="7">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="9">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="10">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="5">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="2">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="8">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8">#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -68,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -361,119 +356,23 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>STR_name</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_icon</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR_rewards</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>quest_1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>quest_2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>quest_3</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>quest_4</t>
-  </si>
-  <si>
-    <t>quest_5</t>
-  </si>
-  <si>
-    <t>quest_6</t>
-  </si>
-  <si>
-    <t>quest_7</t>
-  </si>
-  <si>
-    <t>quest_8</t>
-  </si>
-  <si>
-    <t>quest_9</t>
-  </si>
-  <si>
-    <t>quest_10</t>
-  </si>
-  <si>
-    <t>icon_1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>icon_2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>icon_3</t>
-  </si>
-  <si>
-    <t>icon_4</t>
-  </si>
-  <si>
-    <t>icon_5</t>
-  </si>
-  <si>
-    <t>icon_6</t>
-  </si>
-  <si>
-    <t>icon_7</t>
-  </si>
-  <si>
-    <t>icon_8</t>
-  </si>
-  <si>
-    <t>icon_9</t>
-  </si>
-  <si>
-    <t>icon_10</t>
-  </si>
-  <si>
-    <t>INT_star</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>FLOAT_needMinutes</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>resources:wood:10,resources:stone:10,resources:iron:10</t>
-  </si>
-  <si>
-    <t>INT_style</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_star_1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_star_2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_star_3</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_star_4</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_star_5</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_index</t>
+    <t>STR_type</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_value</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLOAT_value</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>dailyQuestsRefreshHours</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>dailyQuestAddStarNeedGemCount</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -484,7 +383,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0\%"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="宋体"/>
@@ -560,13 +459,6 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -630,7 +522,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -679,8 +571,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -694,11 +588,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="46">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -723,6 +614,7 @@
     <cellStyle name="超链接" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -740,6 +632,7 @@
     <cellStyle name="访问过的超链接" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1189,91 +1082,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="20.6640625" style="1"/>
+    <col min="1" max="1" width="26" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1">
-      <c r="A2" s="1">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="B2" s="1">
-        <v>2000</v>
-      </c>
-      <c r="C2" s="1">
-        <v>25000</v>
-      </c>
-      <c r="D2" s="1">
-        <v>25000</v>
-      </c>
-      <c r="E2" s="1">
-        <v>25000</v>
-      </c>
-      <c r="F2" s="1">
-        <v>25000</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>50000</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>100</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="20" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="20" customHeight="1">
+    <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="B4" s="2"/>
     </row>
   </sheetData>
@@ -1290,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1301,158 +1142,159 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="20" customHeight="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="20" customHeight="1">
+      <c r="B3" s="2">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1">
+        <v>300</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="20" customHeight="1">
+      <c r="B4" s="2">
+        <v>300</v>
+      </c>
+      <c r="C4" s="1">
+        <v>600</v>
+      </c>
+      <c r="D4" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="20" customHeight="1">
+        <v>600</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="16384" width="20.6640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
+        <v>1000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D6" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2100</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2800</v>
+      </c>
+      <c r="D8" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3600</v>
+      </c>
+      <c r="D9" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3600</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4500</v>
+      </c>
+      <c r="D10" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4500</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -1469,74 +1311,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="20.6640625" style="1"/>
+    <col min="1" max="1" width="26" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1">
-      <c r="A2" s="1">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="B2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1000</v>
-      </c>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -1552,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView showRuler="0" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1563,63 +1371,81 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C2" s="1">
-        <v>1000</v>
+        <v>25000</v>
       </c>
       <c r="D2" s="1">
-        <v>1000</v>
+        <v>25000</v>
       </c>
       <c r="E2" s="1">
-        <v>1000</v>
+        <v>25000</v>
       </c>
       <c r="F2" s="1">
-        <v>1000</v>
+        <v>25000</v>
       </c>
       <c r="G2" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
-        <v>1000</v>
+        <v>50000</v>
       </c>
       <c r="I2" s="1">
-        <v>1000</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>100</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="20" customHeight="1">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="20" customHeight="1">
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -1635,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1646,123 +1472,36 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" ht="20" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1788,93 +1527,6 @@
         <v>1000</v>
       </c>
       <c r="I2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="M2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="N2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="O2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="R2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="S2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="T2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="U2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="V2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="W2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="X2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AL2" s="1">
         <v>1000</v>
       </c>
     </row>
@@ -1892,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1903,51 +1555,63 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="1">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="E2" s="1">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="F2" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
-      <c r="B4" s="2"/>
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1000</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -1963,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1974,126 +1638,236 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:38" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="20" customHeight="1">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="20" customHeight="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>100</v>
-      </c>
-      <c r="C3" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>300</v>
-      </c>
-      <c r="C4" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>600</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="20" customHeight="1">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1500</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="20" customHeight="1">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2100</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2800</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="20" customHeight="1">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3600</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>4500</v>
-      </c>
-      <c r="C11" s="1">
-        <v>100000000</v>
+        <v>1000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -2110,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2121,127 +1895,51 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="20" customHeight="1">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="20" customHeight="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>100</v>
-      </c>
-      <c r="C3" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1">
-      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>300</v>
-      </c>
-      <c r="C4" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>600</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="20" customHeight="1">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1500</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="20" customHeight="1">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2100</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2800</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="20" customHeight="1">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3600</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>4500</v>
-      </c>
-      <c r="C11" s="1">
-        <v>10000</v>
-      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -2259,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2278,9 +1976,6 @@
       <c r="C1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
@@ -2293,9 +1988,6 @@
       <c r="C2" s="1">
         <v>100</v>
       </c>
-      <c r="D2" s="1">
-        <v>50</v>
-      </c>
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
@@ -2307,9 +1999,6 @@
       <c r="C3" s="1">
         <v>300</v>
       </c>
-      <c r="D3" s="1">
-        <v>100</v>
-      </c>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
@@ -2321,9 +2010,6 @@
       <c r="C4" s="1">
         <v>600</v>
       </c>
-      <c r="D4" s="1">
-        <v>150</v>
-      </c>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
@@ -2335,9 +2021,6 @@
       <c r="C5" s="1">
         <v>1000</v>
       </c>
-      <c r="D5" s="1">
-        <v>200</v>
-      </c>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
@@ -2349,9 +2032,6 @@
       <c r="C6" s="1">
         <v>1500</v>
       </c>
-      <c r="D6" s="1">
-        <v>250</v>
-      </c>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
@@ -2363,9 +2043,6 @@
       <c r="C7" s="1">
         <v>2100</v>
       </c>
-      <c r="D7" s="1">
-        <v>300</v>
-      </c>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
@@ -2377,9 +2054,6 @@
       <c r="C8" s="1">
         <v>2800</v>
       </c>
-      <c r="D8" s="1">
-        <v>350</v>
-      </c>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
@@ -2391,9 +2065,6 @@
       <c r="C9" s="1">
         <v>3600</v>
       </c>
-      <c r="D9" s="1">
-        <v>400</v>
-      </c>
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
@@ -2405,9 +2076,6 @@
       <c r="C10" s="1">
         <v>4500</v>
       </c>
-      <c r="D10" s="1">
-        <v>450</v>
-      </c>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
@@ -2417,10 +2085,7 @@
         <v>4500</v>
       </c>
       <c r="C11" s="1">
-        <v>10000</v>
-      </c>
-      <c r="D11" s="1">
-        <v>500</v>
+        <v>100000000</v>
       </c>
     </row>
   </sheetData>
@@ -2439,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2450,157 +2115,124 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>98</v>
+      <c r="C2" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>98</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1">
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>98</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>300</v>
+      </c>
+      <c r="C4" s="1">
+        <v>600</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>98</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>600</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>98</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>98</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2100</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>98</v>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2100</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2800</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>98</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3600</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>98</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3600</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4500</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>98</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4500</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify configs add building to 40 and bugfix
</commit_message>
<xml_diff>
--- a/gameData/shared/PlayerInitData.xlsx
+++ b/gameData/shared/PlayerInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="1660" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="8360" yWindow="1440" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="24" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="82">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -385,6 +385,10 @@
   </si>
   <si>
     <t>militaryTechnologyMaxLevel</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>buildingMaxLevel</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1110,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1169,6 +1173,14 @@
       </c>
       <c r="B6" s="1">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish dev of gacha
</commit_message>
<xml_diff>
--- a/gameData/shared/PlayerInitData.xlsx
+++ b/gameData/shared/PlayerInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="2960" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="6540" yWindow="21760" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="24" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="97">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -433,6 +433,22 @@
   </si>
   <si>
     <t>龙复活需要的时间</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>casinoTokenNeededPerNormalGacha</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>普通gacha一次需要多少赌币</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>高级gacha一次需要多少赌币</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>casinoTokenNeededPerAdvancedGacha</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -582,7 +598,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -597,6 +613,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -667,7 +685,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="66">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -702,6 +720,7 @@
     <cellStyle name="超链接" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -729,6 +748,7 @@
     <cellStyle name="访问过的超链接" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1178,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1321,6 +1341,28 @@
       </c>
       <c r="C12" s="1" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="1">
+        <v>100</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first iap rewards support
</commit_message>
<xml_diff>
--- a/gameData/shared/PlayerInitData.xlsx
+++ b/gameData/shared/PlayerInitData.xlsx
@@ -4,53 +4,58 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9220" yWindow="1480" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="5580" yWindow="3700" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="24" r:id="rId1"/>
     <sheet name="floatInit" sheetId="25" r:id="rId2"/>
-    <sheet name="resources" sheetId="2" r:id="rId3"/>
-    <sheet name="materials" sheetId="15" r:id="rId4"/>
-    <sheet name="soldierMaterials" sheetId="19" r:id="rId5"/>
-    <sheet name="dragonMaterials" sheetId="20" r:id="rId6"/>
-    <sheet name="houses" sheetId="18" r:id="rId7"/>
-    <sheet name="playerLevel" sheetId="21" r:id="rId8"/>
-    <sheet name="vipLevel" sheetId="22" r:id="rId9"/>
-    <sheet name="collectLevel" sheetId="23" r:id="rId10"/>
+    <sheet name="stringInit" sheetId="26" r:id="rId3"/>
+    <sheet name="resources" sheetId="2" r:id="rId4"/>
+    <sheet name="materials" sheetId="15" r:id="rId5"/>
+    <sheet name="soldierMaterials" sheetId="19" r:id="rId6"/>
+    <sheet name="dragonMaterials" sheetId="20" r:id="rId7"/>
+    <sheet name="houses" sheetId="18" r:id="rId8"/>
+    <sheet name="playerLevel" sheetId="21" r:id="rId9"/>
+    <sheet name="vipLevel" sheetId="22" r:id="rId10"/>
+    <sheet name="collectLevel" sheetId="23" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="9">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="10">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="6">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="1">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="6">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="7">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="8">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="9">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="10">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="1">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="7">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="8">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="9">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="5">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="1">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="6">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="7">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="8">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="10">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="1">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="7">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="8">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="9">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="5">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="1">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="6">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="7">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="8">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="10">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="1">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="7">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="8">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="5">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="9">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="5">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="1">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="6">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="7">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="4">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="8">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8">#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -63,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="106">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -472,6 +477,18 @@
   </si>
   <si>
     <t>龙的行军速度</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_value</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>resource:woodClass_3:1,resource:stoneClass_3:1,resource:ironClass_3:1,resource:foodClass_3:1,resource:coinClass_2:1,resource:casinoTokenClass_1:1,speedup:speedup_3:2,speedup:speedup_4:1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>firstIAPRewards</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -621,7 +638,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="70">
+  <cellStyleXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -636,6 +653,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -715,7 +738,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="70">
+  <cellStyles count="76">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -753,6 +776,9 @@
     <cellStyle name="超链接" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -783,6 +809,9 @@
     <cellStyle name="访问过的超链接" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1234,7 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1423,6 +1452,153 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="20.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>300</v>
+      </c>
+      <c r="C4" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>600</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2100</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3600</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4500</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -1650,6 +1826,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="20.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="20" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="B3" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="D1" workbookViewId="0">
@@ -1742,89 +1964,6 @@
     </row>
     <row r="4" spans="1:12" ht="20" customHeight="1">
       <c r="B4" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="16384" width="20.6640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="20" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1000</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -1843,7 +1982,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1856,28 +1995,28 @@
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20" customHeight="1">
@@ -1922,6 +2061,89 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="20.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="20" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="20" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
@@ -2130,7 +2352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -2201,7 +2423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
@@ -3639,151 +3861,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="16384" width="20.6640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="20" customHeight="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="20" customHeight="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>100</v>
-      </c>
-      <c r="C3" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>300</v>
-      </c>
-      <c r="C4" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>600</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="20" customHeight="1">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1500</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="20" customHeight="1">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2100</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2800</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="20" customHeight="1">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3600</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>4500</v>
-      </c>
-      <c r="C11" s="1">
-        <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
dev of daily tasks
</commit_message>
<xml_diff>
--- a/gameData/shared/PlayerInitData.xlsx
+++ b/gameData/shared/PlayerInitData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="3700" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="2"/>
+    <workbookView xWindow="6480" yWindow="21740" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="intInit" sheetId="24" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="110">
   <si>
     <t>INT_gem</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -489,6 +489,22 @@
   </si>
   <si>
     <t>firstIAPRewards</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>empireRiseDailyTaskRewards</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>conquerorDailyTaskRewards</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>brotherClubDailyTaskRewards</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>growUpDailyTaskRewards</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -638,7 +654,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="76">
+  <cellStyleXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -653,6 +669,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -738,7 +758,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="76">
+  <cellStyles count="80">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -779,6 +799,8 @@
     <cellStyle name="超链接" xfId="70" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="78" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -812,6 +834,8 @@
     <cellStyle name="访问过的超链接" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1826,10 +1850,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1856,7 +1880,36 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1">
-      <c r="B3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>

</xml_diff>